<commit_message>
HTML editado telas inicial, registro de usuário e cadastro de projeto
</commit_message>
<xml_diff>
--- a/lancerJob/Arquivos do Projeto/database.xlsx
+++ b/lancerJob/Arquivos do Projeto/database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Treinamento.MW7OOS8GMAYAC1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\treinamento\git\lancerjobs2\lancerJob\Arquivos do Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>Cadastro</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>ranking</t>
+  </si>
+  <si>
+    <t>HMTL (interface pura)</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -467,164 +473,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
@@ -632,7 +639,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
@@ -640,50 +647,50 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
@@ -691,30 +698,30 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
@@ -722,16 +729,24 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>35</v>
+        <v>20</v>
+      </c>
+      <c r="C47" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>